<commit_message>
Response and Script Updated
</commit_message>
<xml_diff>
--- a/ParticipantOverviewRecord.xlsx
+++ b/ParticipantOverviewRecord.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Lectures" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tracking!$B$4:$L$256</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tracking!$B$4:$L$257</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="274">
   <si>
     <t>Participant overview record for the study:</t>
   </si>
@@ -393,6 +393,15 @@
     <t>kamal.sharma@stud.fra-uas.de, hafiz.ali25@stud.fra-uas.de, ranjit.khude@stud.fra-uas.de, tanishka.agale@stud.fra-uas.de, rency.padasala@stud.fra-uas.de</t>
   </si>
   <si>
+    <t>Jemil</t>
+  </si>
+  <si>
+    <t>Mangukiya</t>
+  </si>
+  <si>
+    <t>jemil.mangukiya@stud.fra-uas.de</t>
+  </si>
+  <si>
     <t>MOHIT ANIL</t>
   </si>
   <si>
@@ -730,6 +739,99 @@
   </si>
   <si>
     <t>kamal.sharma@stud.fra-uas.de, hafiz.ali48@stud.fra-uas.de, ranjit.khude@stud.fra-uas.de, tanishka.agale@stud.fra-uas.de, rency.padasala@stud.fra-uas.de</t>
+  </si>
+  <si>
+    <t>Amit</t>
+  </si>
+  <si>
+    <t>Sadhu</t>
+  </si>
+  <si>
+    <t>amit.sadhu@stud.fra-uas.de</t>
+  </si>
+  <si>
+    <t>kaival</t>
+  </si>
+  <si>
+    <t>Akbari</t>
+  </si>
+  <si>
+    <t>kaival.akbari@stud.fra-uas.de</t>
+  </si>
+  <si>
+    <t>Ramya</t>
+  </si>
+  <si>
+    <t>Sai Murali</t>
+  </si>
+  <si>
+    <t>ramya.sai-murali@stud.fra-uas.de</t>
+  </si>
+  <si>
+    <t>Danish</t>
+  </si>
+  <si>
+    <t>danish.ali@stud.fra-uas.de</t>
+  </si>
+  <si>
+    <t>kamal.sharma@stud.fra-uas.de, hafiz.ali49@stud.fra-uas.de, ranjit.khude@stud.fra-uas.de, tanishka.agale@stud.fra-uas.de, rency.padasala@stud.fra-uas.de</t>
+  </si>
+  <si>
+    <t>Afif Ullah</t>
+  </si>
+  <si>
+    <t>Khan</t>
+  </si>
+  <si>
+    <t>afif.khan@stud.fra-uas.de</t>
+  </si>
+  <si>
+    <t>kamal.sharma@stud.fra-uas.de, hafiz.ali50@stud.fra-uas.de, ranjit.khude@stud.fra-uas.de, tanishka.agale@stud.fra-uas.de, rency.padasala@stud.fra-uas.de</t>
+  </si>
+  <si>
+    <t>Nouman</t>
+  </si>
+  <si>
+    <t>Tahir</t>
+  </si>
+  <si>
+    <t>nouman.tahir@stud.fra-uas.de</t>
+  </si>
+  <si>
+    <t>kamal.sharma@stud.fra-uas.de, hafiz.ali51@stud.fra-uas.de, ranjit.khude@stud.fra-uas.de, tanishka.agale@stud.fra-uas.de, rency.padasala@stud.fra-uas.de</t>
+  </si>
+  <si>
+    <t>Naqeeb</t>
+  </si>
+  <si>
+    <t>naqeeb.ahmed@stud.fra-uas.de</t>
+  </si>
+  <si>
+    <t>kamal.sharma@stud.fra-uas.de, hafiz.ali52@stud.fra-uas.de, ranjit.khude@stud.fra-uas.de, tanishka.agale@stud.fra-uas.de, rency.padasala@stud.fra-uas.de</t>
+  </si>
+  <si>
+    <t>Muhammad Furqan</t>
+  </si>
+  <si>
+    <t>Shafique</t>
+  </si>
+  <si>
+    <t>muhammad.shafique@stud.fra-uas.de</t>
+  </si>
+  <si>
+    <t>kamal.sharma@stud.fra-uas.de, hafiz.ali53@stud.fra-uas.de, ranjit.khude@stud.fra-uas.de, tanishka.agale@stud.fra-uas.de, rency.padasala@stud.fra-uas.de</t>
+  </si>
+  <si>
+    <t>Hamza</t>
+  </si>
+  <si>
+    <t>Asaad</t>
+  </si>
+  <si>
+    <t>hamza.asaad@stud.fra-uas.de</t>
+  </si>
+  <si>
+    <t>kamal.sharma@stud.fra-uas.de, hafiz.ali54@stud.fra-uas.de, ranjit.khude@stud.fra-uas.de, tanishka.agale@stud.fra-uas.de, rency.padasala@stud.fra-uas.de</t>
   </si>
   <si>
     <t>Usability Engineering (Bachelor)</t>
@@ -1455,7 +1557,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1527,6 +1629,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1535,15 +1643,6 @@
     </xf>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1686,7 +1785,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Matrikelnummern" displayName="Matrikelnummern" ref="A4:B99999" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Matrikelnummern" displayName="Matrikelnummern" ref="A4:B100000" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Study ID/Imma. #" dataDxfId="0"/>
     <tableColumn id="2" name="Firstname"/>
@@ -1953,10 +2052,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M256"/>
+  <dimension ref="A1:M257"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="13.2"/>
@@ -1988,10 +2087,10 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="H1" s="11"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" s="3" customFormat="1" ht="28.35" customHeight="1" spans="1:12">
       <c r="A2" s="12" t="s">
@@ -2004,10 +2103,10 @@
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="H2" s="14"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
     </row>
     <row r="3" s="4" customFormat="1" ht="57.75" customHeight="1" spans="1:12">
       <c r="A3" s="15" t="s">
@@ -2144,7 +2243,7 @@
       <c r="L6" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M6" s="30" t="s">
+      <c r="M6" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2185,7 +2284,7 @@
       <c r="L7" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="30" t="s">
+      <c r="M7" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2226,7 +2325,7 @@
       <c r="L8" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M8" s="30" t="s">
+      <c r="M8" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2267,7 +2366,7 @@
       <c r="L9" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2308,7 +2407,7 @@
       <c r="L10" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M10" s="30" t="s">
+      <c r="M10" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2349,7 +2448,7 @@
       <c r="L11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="30" t="s">
+      <c r="M11" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2390,7 +2489,7 @@
       <c r="L12" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M12" s="30" t="s">
+      <c r="M12" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2431,7 +2530,7 @@
       <c r="L13" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M13" s="30" t="s">
+      <c r="M13" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2472,7 +2571,7 @@
       <c r="L14" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M14" s="30" t="s">
+      <c r="M14" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2513,7 +2612,7 @@
       <c r="L15" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M15" s="30" t="s">
+      <c r="M15" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2554,7 +2653,7 @@
       <c r="L16" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M16" s="30" t="s">
+      <c r="M16" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2595,7 +2694,7 @@
       <c r="L17" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M17" s="30" t="s">
+      <c r="M17" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2636,7 +2735,7 @@
       <c r="L18" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M18" s="30" t="s">
+      <c r="M18" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2677,7 +2776,7 @@
       <c r="L19" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M19" s="30" t="s">
+      <c r="M19" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2718,7 +2817,7 @@
       <c r="L20" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M20" s="30" t="s">
+      <c r="M20" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2759,7 +2858,7 @@
       <c r="L21" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M21" s="30" t="s">
+      <c r="M21" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2800,7 +2899,7 @@
       <c r="L22" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M22" s="30" t="s">
+      <c r="M22" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2841,7 +2940,7 @@
       <c r="L23" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M23" s="30" t="s">
+      <c r="M23" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2882,7 +2981,7 @@
       <c r="L24" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M24" s="30" t="s">
+      <c r="M24" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2923,7 +3022,7 @@
       <c r="L25" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M25" s="30" t="s">
+      <c r="M25" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2964,7 +3063,7 @@
       <c r="L26" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M26" s="30" t="s">
+      <c r="M26" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3005,7 +3104,7 @@
       <c r="L27" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M27" s="30" t="s">
+      <c r="M27" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3046,7 +3145,7 @@
       <c r="L28" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M28" s="30" t="s">
+      <c r="M28" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3087,28 +3186,28 @@
       <c r="L29" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M29" s="30" t="s">
+      <c r="M29" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="30" ht="30.6" spans="1:13">
       <c r="A30" s="17">
-        <v>1569058</v>
-      </c>
-      <c r="B30" s="22" t="s">
+        <v>1612558</v>
+      </c>
+      <c r="B30" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="17" t="s">
         <v>121</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="17" t="s">
         <v>19</v>
       </c>
       <c r="F30" s="20">
-        <v>45881</v>
+        <v>45882</v>
       </c>
       <c r="G30" s="23">
         <v>1</v>
@@ -3117,7 +3216,7 @@
         <v>20</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="J30" s="19" t="s">
         <v>22</v>
@@ -3128,22 +3227,22 @@
       <c r="L30" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M30" s="30" t="s">
+      <c r="M30" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="31" ht="30.6" spans="1:13">
       <c r="A31" s="17">
-        <v>1593860</v>
-      </c>
-      <c r="B31" s="17" t="s">
+        <v>1569058</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="D31" s="17" t="s">
         <v>125</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>126</v>
       </c>
       <c r="E31" s="19" t="s">
         <v>19</v>
@@ -3158,7 +3257,7 @@
         <v>20</v>
       </c>
       <c r="I31" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J31" s="19" t="s">
         <v>22</v>
@@ -3169,38 +3268,38 @@
       <c r="L31" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M31" s="30" t="s">
+      <c r="M31" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="32" ht="30.6" spans="1:13">
       <c r="A32" s="17">
-        <v>1542420</v>
-      </c>
-      <c r="B32" s="22" t="s">
+        <v>1593860</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="D32" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="E32" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="20">
+        <v>45881</v>
+      </c>
+      <c r="G32" s="23">
+        <v>1</v>
+      </c>
+      <c r="H32" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="E32" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" s="20">
-        <v>45882</v>
-      </c>
-      <c r="G32" s="23">
-        <v>1</v>
-      </c>
-      <c r="H32" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I32" s="19" t="s">
-        <v>131</v>
-      </c>
       <c r="J32" s="19" t="s">
         <v>22</v>
       </c>
@@ -3210,22 +3309,22 @@
       <c r="L32" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M32" s="30" t="s">
+      <c r="M32" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="33" ht="30.6" spans="1:13">
       <c r="A33" s="17">
-        <v>1581975</v>
-      </c>
-      <c r="B33" s="17" t="s">
+        <v>1542420</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="D33" s="17" t="s">
         <v>133</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>134</v>
       </c>
       <c r="E33" s="19" t="s">
         <v>19</v>
@@ -3240,33 +3339,33 @@
         <v>20</v>
       </c>
       <c r="I33" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="J33" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K33" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L33" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M33" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" ht="30.6" spans="1:13">
+      <c r="A34" s="17">
+        <v>1581975</v>
+      </c>
+      <c r="B34" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="J33" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="K33" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="L33" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="M33" s="30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" ht="30.6" spans="1:13">
-      <c r="A34" s="6">
-        <v>1542037</v>
-      </c>
-      <c r="B34" s="22" t="s">
+      <c r="C34" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="D34" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="D34" s="24" t="s">
-        <v>138</v>
       </c>
       <c r="E34" s="19" t="s">
         <v>19</v>
@@ -3281,33 +3380,33 @@
         <v>20</v>
       </c>
       <c r="I34" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="J34" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K34" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L34" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M34" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" ht="30.6" spans="1:13">
+      <c r="A35" s="6">
+        <v>1542037</v>
+      </c>
+      <c r="B35" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="J34" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="K34" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="L34" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="M34" s="30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" ht="30.6" spans="1:13">
-      <c r="A35" s="17">
-        <v>1541829</v>
-      </c>
-      <c r="B35" s="22" t="s">
+      <c r="C35" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="D35" s="24" t="s">
         <v>141</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>142</v>
       </c>
       <c r="E35" s="19" t="s">
         <v>19</v>
@@ -3322,7 +3421,7 @@
         <v>20</v>
       </c>
       <c r="I35" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J35" s="19" t="s">
         <v>22</v>
@@ -3333,22 +3432,22 @@
       <c r="L35" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M35" s="30" t="s">
+      <c r="M35" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="36" ht="30.6" spans="1:13">
       <c r="A36" s="17">
-        <v>1523447</v>
+        <v>1541829</v>
       </c>
       <c r="B36" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="D36" s="17" t="s">
         <v>145</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>146</v>
       </c>
       <c r="E36" s="19" t="s">
         <v>19</v>
@@ -3363,7 +3462,7 @@
         <v>20</v>
       </c>
       <c r="I36" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J36" s="19" t="s">
         <v>22</v>
@@ -3374,22 +3473,22 @@
       <c r="L36" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M36" s="30" t="s">
+      <c r="M36" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="37" ht="30.6" spans="1:13">
       <c r="A37" s="17">
-        <v>1542532</v>
-      </c>
-      <c r="B37" s="17" t="s">
+        <v>1523447</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="C37" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="C37" s="17" t="s">
+      <c r="D37" s="17" t="s">
         <v>149</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>150</v>
       </c>
       <c r="E37" s="19" t="s">
         <v>19</v>
@@ -3404,7 +3503,7 @@
         <v>20</v>
       </c>
       <c r="I37" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J37" s="19" t="s">
         <v>22</v>
@@ -3415,22 +3514,22 @@
       <c r="L37" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M37" s="30" t="s">
+      <c r="M37" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="38" ht="30.6" spans="1:13">
       <c r="A38" s="17">
-        <v>1554018</v>
+        <v>1542532</v>
       </c>
       <c r="B38" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C38" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="D38" s="17" t="s">
         <v>153</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>154</v>
       </c>
       <c r="E38" s="19" t="s">
         <v>19</v>
@@ -3445,7 +3544,7 @@
         <v>20</v>
       </c>
       <c r="I38" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J38" s="19" t="s">
         <v>22</v>
@@ -3456,22 +3555,22 @@
       <c r="L38" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M38" s="30" t="s">
+      <c r="M38" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="39" ht="30.6" spans="1:13">
       <c r="A39" s="17">
-        <v>1552085</v>
+        <v>1554018</v>
       </c>
       <c r="B39" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C39" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="D39" s="17" t="s">
         <v>157</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>158</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>19</v>
@@ -3486,7 +3585,7 @@
         <v>20</v>
       </c>
       <c r="I39" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J39" s="19" t="s">
         <v>22</v>
@@ -3497,19 +3596,19 @@
       <c r="L39" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M39" s="30" t="s">
+      <c r="M39" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="40" ht="30.6" spans="1:13">
       <c r="A40" s="17">
-        <v>1470325</v>
+        <v>1552085</v>
       </c>
       <c r="B40" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C40" s="17" t="s">
         <v>160</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>73</v>
       </c>
       <c r="D40" s="17" t="s">
         <v>161</v>
@@ -3527,7 +3626,7 @@
         <v>20</v>
       </c>
       <c r="I40" s="19" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="J40" s="19" t="s">
         <v>22</v>
@@ -3538,19 +3637,19 @@
       <c r="L40" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M40" s="30" t="s">
+      <c r="M40" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="41" ht="30.6" spans="1:13">
       <c r="A41" s="17">
-        <v>1411818</v>
+        <v>1470325</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="C41" s="17" t="s">
         <v>163</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="D41" s="17" t="s">
         <v>164</v>
@@ -3568,7 +3667,7 @@
         <v>20</v>
       </c>
       <c r="I41" s="19" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="J41" s="19" t="s">
         <v>22</v>
@@ -3579,13 +3678,13 @@
       <c r="L41" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M41" s="30" t="s">
+      <c r="M41" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="42" ht="30.6" spans="1:13">
       <c r="A42" s="17">
-        <v>1522932</v>
+        <v>1411818</v>
       </c>
       <c r="B42" s="17" t="s">
         <v>165</v>
@@ -3609,7 +3708,7 @@
         <v>20</v>
       </c>
       <c r="I42" s="19" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="J42" s="19" t="s">
         <v>22</v>
@@ -3620,13 +3719,13 @@
       <c r="L42" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M42" s="30" t="s">
+      <c r="M42" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="43" ht="30.6" spans="1:13">
       <c r="A43" s="17">
-        <v>1502457</v>
+        <v>1522932</v>
       </c>
       <c r="B43" s="17" t="s">
         <v>168</v>
@@ -3650,7 +3749,7 @@
         <v>20</v>
       </c>
       <c r="I43" s="19" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="J43" s="19" t="s">
         <v>22</v>
@@ -3661,13 +3760,13 @@
       <c r="L43" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M43" s="30" t="s">
+      <c r="M43" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="44" ht="30.6" spans="1:13">
       <c r="A44" s="17">
-        <v>1590108</v>
+        <v>1502457</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>171</v>
@@ -3691,7 +3790,7 @@
         <v>20</v>
       </c>
       <c r="I44" s="19" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="J44" s="19" t="s">
         <v>22</v>
@@ -3702,13 +3801,13 @@
       <c r="L44" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M44" s="30" t="s">
+      <c r="M44" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="45" ht="30.6" spans="1:13">
       <c r="A45" s="17">
-        <v>1613245</v>
+        <v>1590108</v>
       </c>
       <c r="B45" s="17" t="s">
         <v>174</v>
@@ -3732,7 +3831,7 @@
         <v>20</v>
       </c>
       <c r="I45" s="19" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="J45" s="19" t="s">
         <v>22</v>
@@ -3743,22 +3842,22 @@
       <c r="L45" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M45" s="30" t="s">
+      <c r="M45" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="46" ht="30.6" spans="1:13">
       <c r="A46" s="17">
-        <v>1541551</v>
+        <v>1613245</v>
       </c>
       <c r="B46" s="17" t="s">
         <v>177</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>73</v>
+        <v>178</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E46" s="19" t="s">
         <v>19</v>
@@ -3773,7 +3872,7 @@
         <v>20</v>
       </c>
       <c r="I46" s="19" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="J46" s="19" t="s">
         <v>22</v>
@@ -3784,19 +3883,19 @@
       <c r="L46" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M46" s="30" t="s">
+      <c r="M46" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="47" ht="30.6" spans="1:13">
       <c r="A47" s="17">
-        <v>1585733</v>
+        <v>1541551</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>180</v>
+        <v>73</v>
       </c>
       <c r="D47" s="17" t="s">
         <v>181</v>
@@ -3814,7 +3913,7 @@
         <v>20</v>
       </c>
       <c r="I47" s="19" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="J47" s="19" t="s">
         <v>22</v>
@@ -3825,28 +3924,28 @@
       <c r="L47" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M47" s="30" t="s">
+      <c r="M47" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="48" ht="30.6" spans="1:13">
       <c r="A48" s="17">
-        <v>15418415</v>
+        <v>1585733</v>
       </c>
       <c r="B48" s="17" t="s">
         <v>182</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>85</v>
+        <v>183</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E48" s="19" t="s">
         <v>19</v>
       </c>
       <c r="F48" s="20">
-        <v>45883</v>
+        <v>45882</v>
       </c>
       <c r="G48" s="23">
         <v>1</v>
@@ -3855,7 +3954,7 @@
         <v>20</v>
       </c>
       <c r="I48" s="19" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="J48" s="19" t="s">
         <v>22</v>
@@ -3866,22 +3965,22 @@
       <c r="L48" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M48" s="30" t="s">
+      <c r="M48" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="49" ht="30.6" spans="1:13">
       <c r="A49" s="17">
-        <v>1541861</v>
+        <v>15418415</v>
       </c>
       <c r="B49" s="17" t="s">
         <v>185</v>
       </c>
       <c r="C49" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D49" s="17" t="s">
         <v>186</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>187</v>
       </c>
       <c r="E49" s="19" t="s">
         <v>19</v>
@@ -3896,7 +3995,7 @@
         <v>20</v>
       </c>
       <c r="I49" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J49" s="19" t="s">
         <v>22</v>
@@ -3907,22 +4006,22 @@
       <c r="L49" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M49" s="30" t="s">
+      <c r="M49" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="50" ht="30.6" spans="1:13">
       <c r="A50" s="17">
-        <v>1541720</v>
+        <v>1541861</v>
       </c>
       <c r="B50" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="C50" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="D50" s="17" t="s">
         <v>190</v>
-      </c>
-      <c r="D50" s="17" t="s">
-        <v>191</v>
       </c>
       <c r="E50" s="19" t="s">
         <v>19</v>
@@ -3937,7 +4036,7 @@
         <v>20</v>
       </c>
       <c r="I50" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J50" s="19" t="s">
         <v>22</v>
@@ -3948,22 +4047,22 @@
       <c r="L50" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M50" s="30" t="s">
+      <c r="M50" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="51" ht="30.6" spans="1:13">
       <c r="A51" s="17">
-        <v>1553813</v>
+        <v>1541720</v>
       </c>
       <c r="B51" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="C51" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="C51" s="17" t="s">
+      <c r="D51" s="17" t="s">
         <v>194</v>
-      </c>
-      <c r="D51" s="17" t="s">
-        <v>195</v>
       </c>
       <c r="E51" s="19" t="s">
         <v>19</v>
@@ -3978,7 +4077,7 @@
         <v>20</v>
       </c>
       <c r="I51" s="19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J51" s="19" t="s">
         <v>22</v>
@@ -3989,22 +4088,22 @@
       <c r="L51" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M51" s="30" t="s">
+      <c r="M51" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="52" ht="30.6" spans="1:13">
       <c r="A52" s="17">
-        <v>1480221</v>
+        <v>1553813</v>
       </c>
       <c r="B52" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C52" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="C52" s="17" t="s">
+      <c r="D52" s="17" t="s">
         <v>198</v>
-      </c>
-      <c r="D52" s="17" t="s">
-        <v>199</v>
       </c>
       <c r="E52" s="19" t="s">
         <v>19</v>
@@ -4019,7 +4118,7 @@
         <v>20</v>
       </c>
       <c r="I52" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J52" s="19" t="s">
         <v>22</v>
@@ -4030,22 +4129,22 @@
       <c r="L52" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M52" s="30" t="s">
+      <c r="M52" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="53" ht="30.6" spans="1:13">
       <c r="A53" s="17">
-        <v>1543229</v>
+        <v>1480221</v>
       </c>
       <c r="B53" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C53" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="D53" s="17" t="s">
         <v>202</v>
-      </c>
-      <c r="D53" s="17" t="s">
-        <v>203</v>
       </c>
       <c r="E53" s="19" t="s">
         <v>19</v>
@@ -4060,7 +4159,7 @@
         <v>20</v>
       </c>
       <c r="I53" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J53" s="19" t="s">
         <v>22</v>
@@ -4071,22 +4170,22 @@
       <c r="L53" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M53" s="30" t="s">
+      <c r="M53" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="54" ht="30.6" spans="1:13">
       <c r="A54" s="17">
-        <v>1511619</v>
+        <v>1543229</v>
       </c>
       <c r="B54" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="C54" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="D54" s="17" t="s">
         <v>206</v>
-      </c>
-      <c r="D54" s="17" t="s">
-        <v>207</v>
       </c>
       <c r="E54" s="19" t="s">
         <v>19</v>
@@ -4101,7 +4200,7 @@
         <v>20</v>
       </c>
       <c r="I54" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J54" s="19" t="s">
         <v>22</v>
@@ -4112,22 +4211,22 @@
       <c r="L54" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M54" s="30" t="s">
+      <c r="M54" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="55" ht="30.6" spans="1:13">
       <c r="A55" s="17">
-        <v>1511635</v>
+        <v>1511619</v>
       </c>
       <c r="B55" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="C55" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="C55" s="17" t="s">
+      <c r="D55" s="17" t="s">
         <v>210</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>211</v>
       </c>
       <c r="E55" s="19" t="s">
         <v>19</v>
@@ -4142,7 +4241,7 @@
         <v>20</v>
       </c>
       <c r="I55" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J55" s="19" t="s">
         <v>22</v>
@@ -4153,22 +4252,22 @@
       <c r="L55" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M55" s="30" t="s">
+      <c r="M55" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="56" ht="30.6" spans="1:13">
       <c r="A56" s="17">
-        <v>1576443</v>
+        <v>1511635</v>
       </c>
       <c r="B56" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="C56" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="D56" s="17" t="s">
         <v>214</v>
-      </c>
-      <c r="D56" s="17" t="s">
-        <v>215</v>
       </c>
       <c r="E56" s="19" t="s">
         <v>19</v>
@@ -4183,7 +4282,7 @@
         <v>20</v>
       </c>
       <c r="I56" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J56" s="19" t="s">
         <v>22</v>
@@ -4194,22 +4293,22 @@
       <c r="L56" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M56" s="30" t="s">
+      <c r="M56" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="57" ht="30.6" spans="1:13">
       <c r="A57" s="17">
-        <v>1591022</v>
+        <v>1576443</v>
       </c>
       <c r="B57" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="C57" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="C57" s="17" t="s">
+      <c r="D57" s="17" t="s">
         <v>218</v>
-      </c>
-      <c r="D57" s="17" t="s">
-        <v>219</v>
       </c>
       <c r="E57" s="19" t="s">
         <v>19</v>
@@ -4224,7 +4323,7 @@
         <v>20</v>
       </c>
       <c r="I57" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J57" s="19" t="s">
         <v>22</v>
@@ -4235,22 +4334,22 @@
       <c r="L57" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M57" s="30" t="s">
+      <c r="M57" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="58" ht="30.6" spans="1:13">
       <c r="A58" s="17">
-        <v>1543670</v>
+        <v>1591022</v>
       </c>
       <c r="B58" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="C58" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="C58" s="17" t="s">
+      <c r="D58" s="17" t="s">
         <v>222</v>
-      </c>
-      <c r="D58" s="17" t="s">
-        <v>223</v>
       </c>
       <c r="E58" s="19" t="s">
         <v>19</v>
@@ -4265,7 +4364,7 @@
         <v>20</v>
       </c>
       <c r="I58" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J58" s="19" t="s">
         <v>22</v>
@@ -4276,22 +4375,22 @@
       <c r="L58" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M58" s="30" t="s">
+      <c r="M58" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="59" ht="30.6" spans="1:13">
       <c r="A59" s="17">
-        <v>1475773</v>
+        <v>1543670</v>
       </c>
       <c r="B59" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="C59" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="C59" s="17" t="s">
+      <c r="D59" s="17" t="s">
         <v>226</v>
-      </c>
-      <c r="D59" s="17" t="s">
-        <v>227</v>
       </c>
       <c r="E59" s="19" t="s">
         <v>19</v>
@@ -4306,7 +4405,7 @@
         <v>20</v>
       </c>
       <c r="I59" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J59" s="19" t="s">
         <v>22</v>
@@ -4317,22 +4416,22 @@
       <c r="L59" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M59" s="30" t="s">
+      <c r="M59" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="60" ht="30.6" spans="1:13">
       <c r="A60" s="17">
-        <v>1542095</v>
+        <v>1475773</v>
       </c>
       <c r="B60" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="C60" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="D60" s="17" t="s">
         <v>230</v>
-      </c>
-      <c r="D60" s="17" t="s">
-        <v>231</v>
       </c>
       <c r="E60" s="19" t="s">
         <v>19</v>
@@ -4347,953 +4446,1300 @@
         <v>20</v>
       </c>
       <c r="I60" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="J60" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K60" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L60" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M60" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" ht="30.6" spans="1:13">
+      <c r="A61" s="17">
+        <v>1542095</v>
+      </c>
+      <c r="B61" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="J60" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="K60" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="L60" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="M60" s="30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="8"/>
-      <c r="B61" s="25"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="27"/>
-      <c r="G61" s="27"/>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="8"/>
-      <c r="B62" s="25"/>
-      <c r="E62" s="26"/>
-      <c r="F62" s="27"/>
-      <c r="G62" s="27"/>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="8"/>
-      <c r="B63" s="25"/>
-      <c r="E63" s="26"/>
-      <c r="F63" s="27"/>
-      <c r="G63" s="27"/>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="8"/>
-      <c r="B64" s="25"/>
-      <c r="E64" s="26"/>
-      <c r="F64" s="27"/>
-      <c r="G64" s="27"/>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="8"/>
-      <c r="B65" s="25"/>
-      <c r="E65" s="26"/>
-      <c r="F65" s="27"/>
-      <c r="G65" s="27"/>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66" s="8"/>
-      <c r="B66" s="25"/>
-      <c r="E66" s="26"/>
-      <c r="F66" s="27"/>
-      <c r="G66" s="27"/>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67" s="8"/>
-      <c r="B67" s="25"/>
-      <c r="E67" s="26"/>
-      <c r="F67" s="27"/>
-      <c r="G67" s="27"/>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68" s="8"/>
-      <c r="B68" s="25"/>
-      <c r="E68" s="26"/>
-      <c r="F68" s="27"/>
-      <c r="G68" s="27"/>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" s="8"/>
-      <c r="B69" s="25"/>
-      <c r="E69" s="26"/>
-      <c r="F69" s="27"/>
-      <c r="G69" s="27"/>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="A70" s="8"/>
-      <c r="B70" s="25"/>
-      <c r="E70" s="26"/>
-      <c r="F70" s="27"/>
-      <c r="G70" s="27"/>
+      <c r="C61" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="E61" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61" s="20">
+        <v>45883</v>
+      </c>
+      <c r="G61" s="23">
+        <v>1</v>
+      </c>
+      <c r="H61" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I61" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="J61" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K61" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L61" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M61" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" ht="30.6" spans="1:13">
+      <c r="A62" s="17">
+        <v>1582448</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F62" s="20">
+        <v>45883</v>
+      </c>
+      <c r="G62" s="23">
+        <v>1</v>
+      </c>
+      <c r="H62" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I62" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="J62" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K62" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L62" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M62" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" ht="30.6" spans="1:13">
+      <c r="A63" s="17">
+        <v>1387256</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D63" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F63" s="20">
+        <v>45884</v>
+      </c>
+      <c r="G63" s="23">
+        <v>1</v>
+      </c>
+      <c r="H63" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I63" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="J63" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K63" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L63" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M63" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" ht="30.6" spans="1:13">
+      <c r="A64" s="17">
+        <v>1584020</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F64" s="20">
+        <v>45884</v>
+      </c>
+      <c r="G64" s="23">
+        <v>1</v>
+      </c>
+      <c r="H64" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I64" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="J64" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K64" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L64" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M64" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" ht="30.6" spans="1:13">
+      <c r="A65" s="17">
+        <v>1541535</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="E65" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F65" s="20">
+        <v>45884</v>
+      </c>
+      <c r="G65" s="23">
+        <v>1</v>
+      </c>
+      <c r="H65" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I65" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="J65" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K65" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L65" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M65" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" ht="30.6" spans="1:13">
+      <c r="A66" s="17">
+        <v>1504761</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="D66" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="E66" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F66" s="20">
+        <v>45884</v>
+      </c>
+      <c r="G66" s="23">
+        <v>1</v>
+      </c>
+      <c r="H66" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I66" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="J66" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K66" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L66" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M66" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" ht="30.6" spans="1:13">
+      <c r="A67" s="17">
+        <v>1503032</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D67" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="E67" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F67" s="20">
+        <v>45885</v>
+      </c>
+      <c r="G67" s="23">
+        <v>1</v>
+      </c>
+      <c r="H67" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I67" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="J67" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K67" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L67" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M67" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" ht="30.6" spans="1:13">
+      <c r="A68" s="17">
+        <v>1505317</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D68" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="E68" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F68" s="20">
+        <v>45885</v>
+      </c>
+      <c r="G68" s="23">
+        <v>1</v>
+      </c>
+      <c r="H68" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I68" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="J68" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K68" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L68" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M68" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" ht="30.6" spans="1:13">
+      <c r="A69" s="17">
+        <v>1521612</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="D69" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="E69" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F69" s="20">
+        <v>45885</v>
+      </c>
+      <c r="G69" s="23">
+        <v>1</v>
+      </c>
+      <c r="H69" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I69" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="J69" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K69" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L69" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M69" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" ht="30.6" spans="1:13">
+      <c r="A70" s="17">
+        <v>1581917</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="D70" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="E70" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F70" s="20">
+        <v>45886</v>
+      </c>
+      <c r="G70" s="23">
+        <v>1</v>
+      </c>
+      <c r="H70" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I70" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="J70" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K70" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L70" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M70" s="24" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="8"/>
-      <c r="B71" s="25"/>
-      <c r="E71" s="26"/>
-      <c r="F71" s="27"/>
-      <c r="G71" s="27"/>
+      <c r="B71" s="27"/>
+      <c r="E71" s="28"/>
+      <c r="F71" s="29"/>
+      <c r="G71" s="29"/>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="8"/>
-      <c r="B72" s="25"/>
-      <c r="E72" s="26"/>
-      <c r="F72" s="27"/>
-      <c r="G72" s="27"/>
+      <c r="B72" s="27"/>
+      <c r="E72" s="28"/>
+      <c r="F72" s="29"/>
+      <c r="G72" s="29"/>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="8"/>
-      <c r="B73" s="25"/>
-      <c r="E73" s="26"/>
-      <c r="F73" s="27"/>
-      <c r="G73" s="27"/>
+      <c r="B73" s="27"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="29"/>
+      <c r="G73" s="29"/>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="8"/>
-      <c r="B74" s="25"/>
-      <c r="E74" s="26"/>
-      <c r="F74" s="27"/>
-      <c r="G74" s="27"/>
+      <c r="B74" s="27"/>
+      <c r="E74" s="28"/>
+      <c r="F74" s="29"/>
+      <c r="G74" s="29"/>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="8"/>
-      <c r="B75" s="25"/>
-      <c r="E75" s="26"/>
-      <c r="F75" s="27"/>
-      <c r="G75" s="27"/>
+      <c r="B75" s="27"/>
+      <c r="E75" s="28"/>
+      <c r="F75" s="29"/>
+      <c r="G75" s="29"/>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="8"/>
-      <c r="B76" s="25"/>
-      <c r="E76" s="26"/>
-      <c r="F76" s="27"/>
-      <c r="G76" s="27"/>
+      <c r="B76" s="27"/>
+      <c r="E76" s="28"/>
+      <c r="F76" s="29"/>
+      <c r="G76" s="29"/>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="8"/>
-      <c r="B77" s="25"/>
-      <c r="E77" s="26"/>
-      <c r="F77" s="27"/>
-      <c r="G77" s="27"/>
+      <c r="B77" s="27"/>
+      <c r="E77" s="28"/>
+      <c r="F77" s="29"/>
+      <c r="G77" s="29"/>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="8"/>
-      <c r="B78" s="25"/>
-      <c r="E78" s="26"/>
-      <c r="F78" s="27"/>
-      <c r="G78" s="27"/>
+      <c r="B78" s="27"/>
+      <c r="E78" s="28"/>
+      <c r="F78" s="29"/>
+      <c r="G78" s="29"/>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="8"/>
-      <c r="B79" s="25"/>
-      <c r="E79" s="26"/>
-      <c r="F79" s="27"/>
-      <c r="G79" s="27"/>
+      <c r="B79" s="27"/>
+      <c r="E79" s="28"/>
+      <c r="F79" s="29"/>
+      <c r="G79" s="29"/>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="8"/>
-      <c r="B80" s="25"/>
-      <c r="E80" s="26"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="27"/>
+      <c r="B80" s="27"/>
+      <c r="E80" s="28"/>
+      <c r="F80" s="29"/>
+      <c r="G80" s="29"/>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="8"/>
-      <c r="B81" s="25"/>
-      <c r="E81" s="26"/>
-      <c r="F81" s="27"/>
-      <c r="G81" s="27"/>
+      <c r="B81" s="27"/>
+      <c r="E81" s="28"/>
+      <c r="F81" s="29"/>
+      <c r="G81" s="29"/>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" s="8"/>
-      <c r="B82" s="25"/>
-      <c r="E82" s="26"/>
-      <c r="F82" s="27"/>
-      <c r="G82" s="27"/>
+      <c r="B82" s="27"/>
+      <c r="E82" s="28"/>
+      <c r="F82" s="29"/>
+      <c r="G82" s="29"/>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="8"/>
-      <c r="B83" s="25"/>
-      <c r="E83" s="26"/>
-      <c r="F83" s="27"/>
-      <c r="G83" s="27"/>
+      <c r="B83" s="27"/>
+      <c r="E83" s="28"/>
+      <c r="F83" s="29"/>
+      <c r="G83" s="29"/>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" s="8"/>
-      <c r="B84" s="25"/>
-      <c r="E84" s="26"/>
-      <c r="F84" s="27"/>
-      <c r="G84" s="27"/>
+      <c r="B84" s="27"/>
+      <c r="E84" s="28"/>
+      <c r="F84" s="29"/>
+      <c r="G84" s="29"/>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="8"/>
-      <c r="B85" s="25"/>
-      <c r="E85" s="26"/>
-      <c r="F85" s="27"/>
-      <c r="G85" s="27"/>
+      <c r="B85" s="27"/>
+      <c r="E85" s="28"/>
+      <c r="F85" s="29"/>
+      <c r="G85" s="29"/>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" s="8"/>
-      <c r="B86" s="25"/>
-      <c r="E86" s="26"/>
-      <c r="F86" s="27"/>
-      <c r="G86" s="27"/>
+      <c r="B86" s="27"/>
+      <c r="E86" s="28"/>
+      <c r="F86" s="29"/>
+      <c r="G86" s="29"/>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" s="8"/>
-      <c r="B87" s="25"/>
-      <c r="E87" s="26"/>
-      <c r="F87" s="27"/>
-      <c r="G87" s="27"/>
+      <c r="B87" s="27"/>
+      <c r="E87" s="28"/>
+      <c r="F87" s="29"/>
+      <c r="G87" s="29"/>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" s="8"/>
-      <c r="B88" s="25"/>
-      <c r="E88" s="26"/>
-      <c r="F88" s="27"/>
-      <c r="G88" s="27"/>
+      <c r="B88" s="27"/>
+      <c r="E88" s="28"/>
+      <c r="F88" s="29"/>
+      <c r="G88" s="29"/>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" s="8"/>
-      <c r="B89" s="25"/>
-      <c r="E89" s="26"/>
-      <c r="F89" s="27"/>
-      <c r="G89" s="27"/>
+      <c r="B89" s="27"/>
+      <c r="E89" s="28"/>
+      <c r="F89" s="29"/>
+      <c r="G89" s="29"/>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="8"/>
-      <c r="B90" s="25"/>
-      <c r="E90" s="26"/>
-      <c r="F90" s="27"/>
-      <c r="G90" s="27"/>
+      <c r="B90" s="27"/>
+      <c r="E90" s="28"/>
+      <c r="F90" s="29"/>
+      <c r="G90" s="29"/>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" s="8"/>
-      <c r="B91" s="25"/>
-      <c r="E91" s="26"/>
-      <c r="F91" s="27"/>
-      <c r="G91" s="27"/>
+      <c r="B91" s="27"/>
+      <c r="E91" s="28"/>
+      <c r="F91" s="29"/>
+      <c r="G91" s="29"/>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" s="8"/>
-      <c r="B92" s="25"/>
-      <c r="E92" s="26"/>
-      <c r="F92" s="27"/>
-      <c r="G92" s="27"/>
+      <c r="B92" s="27"/>
+      <c r="E92" s="28"/>
+      <c r="F92" s="29"/>
+      <c r="G92" s="29"/>
     </row>
     <row r="93" spans="1:7">
       <c r="A93" s="8"/>
-      <c r="B93" s="25"/>
-      <c r="E93" s="26"/>
-      <c r="F93" s="27"/>
-      <c r="G93" s="27"/>
+      <c r="B93" s="27"/>
+      <c r="E93" s="28"/>
+      <c r="F93" s="29"/>
+      <c r="G93" s="29"/>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="8"/>
-      <c r="B94" s="25"/>
-      <c r="E94" s="26"/>
-      <c r="F94" s="27"/>
-      <c r="G94" s="27"/>
+      <c r="B94" s="27"/>
+      <c r="E94" s="28"/>
+      <c r="F94" s="29"/>
+      <c r="G94" s="29"/>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" s="8"/>
-      <c r="B95" s="25"/>
-      <c r="E95" s="26"/>
-      <c r="F95" s="27"/>
-      <c r="G95" s="27"/>
+      <c r="B95" s="27"/>
+      <c r="E95" s="28"/>
+      <c r="F95" s="29"/>
+      <c r="G95" s="29"/>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="8"/>
-      <c r="B96" s="25"/>
-      <c r="E96" s="26"/>
-      <c r="F96" s="27"/>
-      <c r="G96" s="27"/>
+      <c r="B96" s="27"/>
+      <c r="E96" s="28"/>
+      <c r="F96" s="29"/>
+      <c r="G96" s="29"/>
     </row>
     <row r="97" spans="1:7">
       <c r="A97" s="8"/>
-      <c r="B97" s="25"/>
-      <c r="E97" s="26"/>
-      <c r="F97" s="27"/>
-      <c r="G97" s="27"/>
+      <c r="B97" s="27"/>
+      <c r="E97" s="28"/>
+      <c r="F97" s="29"/>
+      <c r="G97" s="29"/>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" s="8"/>
-      <c r="B98" s="25"/>
-      <c r="E98" s="26"/>
-      <c r="F98" s="27"/>
-      <c r="G98" s="27"/>
+      <c r="B98" s="27"/>
+      <c r="E98" s="28"/>
+      <c r="F98" s="29"/>
+      <c r="G98" s="29"/>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" s="8"/>
-      <c r="B99" s="25"/>
-      <c r="E99" s="26"/>
-      <c r="F99" s="27"/>
-      <c r="G99" s="27"/>
+      <c r="B99" s="27"/>
+      <c r="E99" s="28"/>
+      <c r="F99" s="29"/>
+      <c r="G99" s="29"/>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" s="8"/>
-      <c r="B100" s="25"/>
-      <c r="E100" s="26"/>
-      <c r="F100" s="27"/>
-      <c r="G100" s="27"/>
+      <c r="B100" s="27"/>
+      <c r="E100" s="28"/>
+      <c r="F100" s="29"/>
+      <c r="G100" s="29"/>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" s="8"/>
-      <c r="B101" s="25"/>
-      <c r="E101" s="26"/>
-      <c r="F101" s="27"/>
-      <c r="G101" s="27"/>
+      <c r="B101" s="27"/>
+      <c r="E101" s="28"/>
+      <c r="F101" s="29"/>
+      <c r="G101" s="29"/>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" s="8"/>
-      <c r="B102" s="25"/>
-      <c r="E102" s="26"/>
-      <c r="F102" s="27"/>
-      <c r="G102" s="27"/>
+      <c r="B102" s="27"/>
+      <c r="E102" s="28"/>
+      <c r="F102" s="29"/>
+      <c r="G102" s="29"/>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="8"/>
-      <c r="B103" s="25"/>
-      <c r="E103" s="26"/>
-      <c r="F103" s="27"/>
-      <c r="G103" s="27"/>
+      <c r="B103" s="27"/>
+      <c r="E103" s="28"/>
+      <c r="F103" s="29"/>
+      <c r="G103" s="29"/>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" s="8"/>
-      <c r="B104" s="25"/>
-      <c r="E104" s="26"/>
-      <c r="F104" s="27"/>
-      <c r="G104" s="27"/>
-    </row>
-    <row r="105" spans="1:5">
+      <c r="B104" s="27"/>
+      <c r="E104" s="28"/>
+      <c r="F104" s="29"/>
+      <c r="G104" s="29"/>
+    </row>
+    <row r="105" spans="1:7">
       <c r="A105" s="8"/>
-      <c r="E105" s="31"/>
+      <c r="B105" s="27"/>
+      <c r="E105" s="28"/>
+      <c r="F105" s="29"/>
+      <c r="G105" s="29"/>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="8"/>
-      <c r="E106" s="31"/>
+      <c r="E106" s="30"/>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="8"/>
-      <c r="E107" s="31"/>
+      <c r="E107" s="30"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="8"/>
-      <c r="E108" s="31"/>
+      <c r="E108" s="30"/>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="8"/>
-      <c r="E109" s="31"/>
+      <c r="E109" s="30"/>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="8"/>
-      <c r="E110" s="31"/>
+      <c r="E110" s="30"/>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="8"/>
-      <c r="E111" s="31"/>
+      <c r="E111" s="30"/>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="8"/>
-      <c r="E112" s="31"/>
+      <c r="E112" s="30"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="8"/>
-      <c r="E113" s="31"/>
+      <c r="E113" s="30"/>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="8"/>
-      <c r="E114" s="31"/>
+      <c r="E114" s="30"/>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="8"/>
-      <c r="E115" s="31"/>
+      <c r="E115" s="30"/>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="8"/>
-      <c r="E116" s="31"/>
+      <c r="E116" s="30"/>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="8"/>
-      <c r="E117" s="31"/>
+      <c r="E117" s="30"/>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="8"/>
-      <c r="E118" s="31"/>
+      <c r="E118" s="30"/>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="8"/>
-      <c r="E119" s="31"/>
+      <c r="E119" s="30"/>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="8"/>
-      <c r="E120" s="31"/>
+      <c r="E120" s="30"/>
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="8"/>
-      <c r="E121" s="31"/>
+      <c r="E121" s="30"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="8"/>
-      <c r="E122" s="31"/>
+      <c r="E122" s="30"/>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="8"/>
-      <c r="E123" s="31"/>
+      <c r="E123" s="30"/>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="8"/>
-      <c r="E124" s="31"/>
+      <c r="E124" s="30"/>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="8"/>
-      <c r="E125" s="31"/>
+      <c r="E125" s="30"/>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="8"/>
-      <c r="E126" s="31"/>
+      <c r="E126" s="30"/>
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="8"/>
-      <c r="E127" s="31"/>
+      <c r="E127" s="30"/>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="8"/>
-      <c r="E128" s="31"/>
+      <c r="E128" s="30"/>
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="8"/>
-      <c r="E129" s="31"/>
+      <c r="E129" s="30"/>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="8"/>
-      <c r="E130" s="31"/>
+      <c r="E130" s="30"/>
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="8"/>
-      <c r="E131" s="31"/>
+      <c r="E131" s="30"/>
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="8"/>
-      <c r="E132" s="31"/>
+      <c r="E132" s="30"/>
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="8"/>
-      <c r="E133" s="31"/>
+      <c r="E133" s="30"/>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="8"/>
-      <c r="E134" s="31"/>
+      <c r="E134" s="30"/>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="8"/>
-      <c r="E135" s="31"/>
+      <c r="E135" s="30"/>
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="8"/>
-      <c r="E136" s="31"/>
+      <c r="E136" s="30"/>
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="8"/>
-      <c r="E137" s="31"/>
+      <c r="E137" s="30"/>
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="8"/>
-      <c r="E138" s="31"/>
+      <c r="E138" s="30"/>
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="8"/>
-      <c r="E139" s="31"/>
+      <c r="E139" s="30"/>
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="8"/>
-      <c r="E140" s="31"/>
+      <c r="E140" s="30"/>
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="8"/>
-      <c r="E141" s="31"/>
+      <c r="E141" s="30"/>
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="8"/>
-      <c r="E142" s="31"/>
+      <c r="E142" s="30"/>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="8"/>
-      <c r="E143" s="31"/>
+      <c r="E143" s="30"/>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="8"/>
-      <c r="E144" s="31"/>
+      <c r="E144" s="30"/>
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="8"/>
-      <c r="E145" s="31"/>
+      <c r="E145" s="30"/>
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="8"/>
-      <c r="E146" s="31"/>
+      <c r="E146" s="30"/>
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="8"/>
-      <c r="E147" s="31"/>
+      <c r="E147" s="30"/>
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="8"/>
-      <c r="E148" s="31"/>
+      <c r="E148" s="30"/>
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="8"/>
-      <c r="E149" s="31"/>
+      <c r="E149" s="30"/>
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="8"/>
-      <c r="E150" s="31"/>
+      <c r="E150" s="30"/>
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="8"/>
-      <c r="E151" s="31"/>
+      <c r="E151" s="30"/>
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="8"/>
-      <c r="E152" s="31"/>
+      <c r="E152" s="30"/>
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="8"/>
-      <c r="E153" s="31"/>
+      <c r="E153" s="30"/>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="8"/>
-      <c r="E154" s="31"/>
+      <c r="E154" s="30"/>
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="8"/>
-      <c r="E155" s="31"/>
+      <c r="E155" s="30"/>
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="8"/>
-      <c r="E156" s="31"/>
+      <c r="E156" s="30"/>
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="8"/>
-      <c r="E157" s="31"/>
+      <c r="E157" s="30"/>
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="8"/>
-      <c r="E158" s="31"/>
+      <c r="E158" s="30"/>
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="8"/>
-      <c r="E159" s="31"/>
+      <c r="E159" s="30"/>
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="8"/>
-      <c r="E160" s="31"/>
+      <c r="E160" s="30"/>
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="8"/>
-      <c r="E161" s="31"/>
+      <c r="E161" s="30"/>
     </row>
     <row r="162" spans="1:5">
       <c r="A162" s="8"/>
-      <c r="E162" s="31"/>
+      <c r="E162" s="30"/>
     </row>
     <row r="163" spans="1:5">
       <c r="A163" s="8"/>
-      <c r="E163" s="31"/>
+      <c r="E163" s="30"/>
     </row>
     <row r="164" spans="1:5">
       <c r="A164" s="8"/>
-      <c r="E164" s="31"/>
+      <c r="E164" s="30"/>
     </row>
     <row r="165" spans="1:5">
       <c r="A165" s="8"/>
-      <c r="E165" s="31"/>
+      <c r="E165" s="30"/>
     </row>
     <row r="166" spans="1:5">
       <c r="A166" s="8"/>
-      <c r="E166" s="31"/>
+      <c r="E166" s="30"/>
     </row>
     <row r="167" spans="1:5">
       <c r="A167" s="8"/>
-      <c r="E167" s="31"/>
+      <c r="E167" s="30"/>
     </row>
     <row r="168" spans="1:5">
       <c r="A168" s="8"/>
-      <c r="E168" s="31"/>
+      <c r="E168" s="30"/>
     </row>
     <row r="169" spans="1:5">
       <c r="A169" s="8"/>
-      <c r="E169" s="31"/>
+      <c r="E169" s="30"/>
     </row>
     <row r="170" spans="1:5">
       <c r="A170" s="8"/>
-      <c r="E170" s="31"/>
+      <c r="E170" s="30"/>
     </row>
     <row r="171" spans="1:5">
       <c r="A171" s="8"/>
-      <c r="E171" s="31"/>
-    </row>
-    <row r="172" spans="1:10">
+      <c r="E171" s="30"/>
+    </row>
+    <row r="172" spans="1:5">
       <c r="A172" s="8"/>
-      <c r="E172" s="31"/>
-      <c r="I172"/>
-      <c r="J172"/>
-    </row>
-    <row r="173" spans="1:5">
+      <c r="E172" s="30"/>
+    </row>
+    <row r="173" spans="1:10">
       <c r="A173" s="8"/>
-      <c r="E173" s="31"/>
+      <c r="E173" s="30"/>
+      <c r="I173"/>
+      <c r="J173"/>
     </row>
     <row r="174" spans="1:5">
       <c r="A174" s="8"/>
-      <c r="E174" s="31"/>
+      <c r="E174" s="30"/>
     </row>
     <row r="175" spans="1:5">
       <c r="A175" s="8"/>
-      <c r="E175" s="31"/>
+      <c r="E175" s="30"/>
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="8"/>
-      <c r="E176" s="31"/>
+      <c r="E176" s="30"/>
     </row>
     <row r="177" spans="1:5">
       <c r="A177" s="8"/>
-      <c r="E177" s="31"/>
+      <c r="E177" s="30"/>
     </row>
     <row r="178" spans="1:5">
       <c r="A178" s="8"/>
-      <c r="E178" s="31"/>
+      <c r="E178" s="30"/>
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="8"/>
-      <c r="E179" s="31"/>
+      <c r="E179" s="30"/>
     </row>
     <row r="180" spans="1:5">
       <c r="A180" s="8"/>
-      <c r="E180" s="31"/>
+      <c r="E180" s="30"/>
     </row>
     <row r="181" spans="1:5">
       <c r="A181" s="8"/>
-      <c r="E181" s="31"/>
+      <c r="E181" s="30"/>
     </row>
     <row r="182" spans="1:5">
       <c r="A182" s="8"/>
-      <c r="E182" s="31"/>
+      <c r="E182" s="30"/>
     </row>
     <row r="183" spans="1:5">
       <c r="A183" s="8"/>
-      <c r="E183" s="31"/>
+      <c r="E183" s="30"/>
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="8"/>
-      <c r="E184" s="31"/>
+      <c r="E184" s="30"/>
     </row>
     <row r="185" spans="1:5">
       <c r="A185" s="8"/>
-      <c r="E185" s="31"/>
+      <c r="E185" s="30"/>
     </row>
     <row r="186" spans="1:5">
       <c r="A186" s="8"/>
-      <c r="E186" s="31"/>
+      <c r="E186" s="30"/>
     </row>
     <row r="187" spans="1:5">
       <c r="A187" s="8"/>
-      <c r="E187" s="31"/>
+      <c r="E187" s="30"/>
     </row>
     <row r="188" spans="1:5">
       <c r="A188" s="8"/>
-      <c r="E188" s="31"/>
+      <c r="E188" s="30"/>
     </row>
     <row r="189" spans="1:5">
       <c r="A189" s="8"/>
-      <c r="E189" s="31"/>
+      <c r="E189" s="30"/>
     </row>
     <row r="190" spans="1:5">
       <c r="A190" s="8"/>
-      <c r="E190" s="31"/>
+      <c r="E190" s="30"/>
     </row>
     <row r="191" spans="1:5">
       <c r="A191" s="8"/>
-      <c r="E191" s="31"/>
+      <c r="E191" s="30"/>
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="8"/>
-      <c r="E192" s="31"/>
+      <c r="E192" s="30"/>
     </row>
     <row r="193" spans="1:5">
       <c r="A193" s="8"/>
-      <c r="E193" s="31"/>
+      <c r="E193" s="30"/>
     </row>
     <row r="194" spans="1:5">
       <c r="A194" s="8"/>
-      <c r="E194" s="31"/>
+      <c r="E194" s="30"/>
     </row>
     <row r="195" spans="1:5">
       <c r="A195" s="8"/>
-      <c r="E195" s="31"/>
+      <c r="E195" s="30"/>
     </row>
     <row r="196" spans="1:5">
       <c r="A196" s="8"/>
-      <c r="E196" s="31"/>
+      <c r="E196" s="30"/>
     </row>
     <row r="197" spans="1:5">
       <c r="A197" s="8"/>
-      <c r="E197" s="31"/>
+      <c r="E197" s="30"/>
     </row>
     <row r="198" spans="1:5">
       <c r="A198" s="8"/>
-      <c r="E198" s="31"/>
+      <c r="E198" s="30"/>
     </row>
     <row r="199" spans="1:5">
       <c r="A199" s="8"/>
-      <c r="E199" s="31"/>
+      <c r="E199" s="30"/>
     </row>
     <row r="200" spans="1:5">
       <c r="A200" s="8"/>
-      <c r="E200" s="31"/>
+      <c r="E200" s="30"/>
     </row>
     <row r="201" spans="1:5">
       <c r="A201" s="8"/>
-      <c r="E201" s="31"/>
+      <c r="E201" s="30"/>
     </row>
     <row r="202" spans="1:5">
       <c r="A202" s="8"/>
-      <c r="E202" s="31"/>
+      <c r="E202" s="30"/>
     </row>
     <row r="203" spans="1:5">
       <c r="A203" s="8"/>
-      <c r="E203" s="31"/>
+      <c r="E203" s="30"/>
     </row>
     <row r="204" spans="1:5">
       <c r="A204" s="8"/>
-      <c r="E204" s="31"/>
+      <c r="E204" s="30"/>
     </row>
     <row r="205" spans="1:5">
       <c r="A205" s="8"/>
-      <c r="E205" s="31"/>
+      <c r="E205" s="30"/>
     </row>
     <row r="206" spans="1:5">
       <c r="A206" s="8"/>
-      <c r="E206" s="31"/>
+      <c r="E206" s="30"/>
     </row>
     <row r="207" spans="1:5">
       <c r="A207" s="8"/>
-      <c r="E207" s="31"/>
+      <c r="E207" s="30"/>
     </row>
     <row r="208" spans="1:5">
       <c r="A208" s="8"/>
-      <c r="E208" s="31"/>
+      <c r="E208" s="30"/>
     </row>
     <row r="209" spans="1:5">
       <c r="A209" s="8"/>
-      <c r="E209" s="31"/>
+      <c r="E209" s="30"/>
     </row>
     <row r="210" spans="1:5">
       <c r="A210" s="8"/>
-      <c r="E210" s="31"/>
+      <c r="E210" s="30"/>
     </row>
     <row r="211" spans="1:5">
       <c r="A211" s="8"/>
-      <c r="E211" s="31"/>
+      <c r="E211" s="30"/>
     </row>
     <row r="212" spans="1:5">
       <c r="A212" s="8"/>
-      <c r="E212" s="31"/>
+      <c r="E212" s="30"/>
     </row>
     <row r="213" spans="1:5">
       <c r="A213" s="8"/>
-      <c r="E213" s="31"/>
+      <c r="E213" s="30"/>
     </row>
     <row r="214" spans="1:5">
       <c r="A214" s="8"/>
-      <c r="E214" s="31"/>
+      <c r="E214" s="30"/>
     </row>
     <row r="215" spans="1:5">
       <c r="A215" s="8"/>
-      <c r="E215" s="31"/>
+      <c r="E215" s="30"/>
     </row>
     <row r="216" spans="1:5">
       <c r="A216" s="8"/>
-      <c r="E216" s="31"/>
+      <c r="E216" s="30"/>
     </row>
     <row r="217" spans="1:5">
       <c r="A217" s="8"/>
-      <c r="E217" s="31"/>
+      <c r="E217" s="30"/>
     </row>
     <row r="218" spans="1:5">
       <c r="A218" s="8"/>
-      <c r="E218" s="31"/>
+      <c r="E218" s="30"/>
     </row>
     <row r="219" spans="1:5">
       <c r="A219" s="8"/>
-      <c r="E219" s="31"/>
+      <c r="E219" s="30"/>
     </row>
     <row r="220" spans="1:5">
       <c r="A220" s="8"/>
-      <c r="E220" s="31"/>
+      <c r="E220" s="30"/>
     </row>
     <row r="221" spans="1:5">
       <c r="A221" s="8"/>
-      <c r="E221" s="31"/>
+      <c r="E221" s="30"/>
     </row>
     <row r="222" spans="1:5">
       <c r="A222" s="8"/>
-      <c r="E222" s="31"/>
+      <c r="E222" s="30"/>
     </row>
     <row r="223" spans="1:5">
       <c r="A223" s="8"/>
-      <c r="E223" s="31"/>
+      <c r="E223" s="30"/>
     </row>
     <row r="224" spans="1:5">
       <c r="A224" s="8"/>
-      <c r="E224" s="31"/>
+      <c r="E224" s="30"/>
     </row>
     <row r="225" spans="1:5">
       <c r="A225" s="8"/>
-      <c r="E225" s="31"/>
+      <c r="E225" s="30"/>
     </row>
     <row r="226" spans="1:5">
       <c r="A226" s="8"/>
-      <c r="E226" s="31"/>
+      <c r="E226" s="30"/>
     </row>
     <row r="227" spans="1:5">
       <c r="A227" s="8"/>
-      <c r="E227" s="31"/>
+      <c r="E227" s="30"/>
     </row>
     <row r="228" spans="1:5">
       <c r="A228" s="8"/>
-      <c r="E228" s="31"/>
+      <c r="E228" s="30"/>
     </row>
     <row r="229" spans="1:5">
       <c r="A229" s="8"/>
-      <c r="E229" s="31"/>
+      <c r="E229" s="30"/>
     </row>
     <row r="230" spans="1:5">
       <c r="A230" s="8"/>
-      <c r="E230" s="31"/>
+      <c r="E230" s="30"/>
     </row>
     <row r="231" spans="1:5">
       <c r="A231" s="8"/>
-      <c r="E231" s="31"/>
+      <c r="E231" s="30"/>
     </row>
     <row r="232" spans="1:5">
       <c r="A232" s="8"/>
-      <c r="E232" s="31"/>
+      <c r="E232" s="30"/>
     </row>
     <row r="233" spans="1:5">
       <c r="A233" s="8"/>
-      <c r="E233" s="31"/>
+      <c r="E233" s="30"/>
     </row>
     <row r="234" spans="1:5">
       <c r="A234" s="8"/>
-      <c r="E234" s="31"/>
+      <c r="E234" s="30"/>
     </row>
     <row r="235" spans="1:5">
       <c r="A235" s="8"/>
-      <c r="E235" s="31"/>
+      <c r="E235" s="30"/>
     </row>
     <row r="236" spans="1:5">
       <c r="A236" s="8"/>
-      <c r="E236" s="31"/>
+      <c r="E236" s="30"/>
     </row>
     <row r="237" spans="1:5">
       <c r="A237" s="8"/>
-      <c r="E237" s="31"/>
+      <c r="E237" s="30"/>
     </row>
     <row r="238" spans="1:5">
       <c r="A238" s="8"/>
-      <c r="E238" s="31"/>
+      <c r="E238" s="30"/>
     </row>
     <row r="239" spans="1:5">
       <c r="A239" s="8"/>
-      <c r="E239" s="31"/>
+      <c r="E239" s="30"/>
     </row>
     <row r="240" spans="1:5">
       <c r="A240" s="8"/>
-      <c r="E240" s="31"/>
+      <c r="E240" s="30"/>
     </row>
     <row r="241" spans="1:5">
       <c r="A241" s="8"/>
-      <c r="E241" s="31"/>
+      <c r="E241" s="30"/>
     </row>
     <row r="242" spans="1:5">
       <c r="A242" s="8"/>
-      <c r="E242" s="31"/>
+      <c r="E242" s="30"/>
     </row>
     <row r="243" spans="1:5">
       <c r="A243" s="8"/>
-      <c r="E243" s="31"/>
+      <c r="E243" s="30"/>
     </row>
     <row r="244" spans="1:5">
       <c r="A244" s="8"/>
-      <c r="E244" s="31"/>
+      <c r="E244" s="30"/>
     </row>
     <row r="245" spans="1:5">
       <c r="A245" s="8"/>
-      <c r="E245" s="31"/>
+      <c r="E245" s="30"/>
     </row>
     <row r="246" spans="1:5">
       <c r="A246" s="8"/>
-      <c r="E246" s="31"/>
+      <c r="E246" s="30"/>
     </row>
     <row r="247" spans="1:5">
       <c r="A247" s="8"/>
-      <c r="E247" s="31"/>
+      <c r="E247" s="30"/>
     </row>
     <row r="248" spans="1:5">
       <c r="A248" s="8"/>
-      <c r="E248" s="31"/>
+      <c r="E248" s="30"/>
     </row>
     <row r="249" spans="1:5">
       <c r="A249" s="8"/>
-      <c r="E249" s="31"/>
+      <c r="E249" s="30"/>
     </row>
     <row r="250" spans="1:5">
       <c r="A250" s="8"/>
-      <c r="E250" s="31"/>
+      <c r="E250" s="30"/>
     </row>
     <row r="251" spans="1:5">
       <c r="A251" s="8"/>
-      <c r="E251" s="31"/>
+      <c r="E251" s="30"/>
     </row>
     <row r="252" spans="1:5">
       <c r="A252" s="8"/>
-      <c r="E252" s="31"/>
+      <c r="E252" s="30"/>
     </row>
     <row r="253" spans="1:5">
       <c r="A253" s="8"/>
-      <c r="E253" s="31"/>
+      <c r="E253" s="30"/>
     </row>
     <row r="254" spans="1:5">
       <c r="A254" s="8"/>
-      <c r="E254" s="31"/>
+      <c r="E254" s="30"/>
     </row>
     <row r="255" spans="1:5">
       <c r="A255" s="8"/>
-      <c r="E255" s="31"/>
+      <c r="E255" s="30"/>
     </row>
     <row r="256" spans="1:5">
       <c r="A256" s="8"/>
-      <c r="E256" s="31"/>
+      <c r="E256" s="30"/>
+    </row>
+    <row r="257" spans="1:5">
+      <c r="A257" s="8"/>
+      <c r="E257" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A3:L3"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G48 G49 G50 G51 G52 G53 G54 G55 G56 G57 G58 G59 G60 F61:F104 G5:G47 G61:G104">
+    <dataValidation type="decimal" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G30 F71:F105 G5:G29 G31:G105">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E46 E47:E60">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K30 K5:K29 K31:K70">
+      <formula1>Lectures!$A$1:$A$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E29 E31:E70">
       <formula1>Lectures!$A$1:$A$8</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K46 K47:K60">
-      <formula1>Lectures!$A$1:$A$10</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -5334,7 +5780,7 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>233</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -5344,32 +5790,32 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>234</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>235</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>236</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>237</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>238</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>